<commit_message>
removed the bug which kept creating a crops.csv in the previsous code
</commit_message>
<xml_diff>
--- a/data/farmers.xlsx
+++ b/data/farmers.xlsx
@@ -61,7 +61,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -125,10 +125,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -450,7 +450,7 @@
     <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -494,7 +494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>